<commit_message>
added fasteners to bill of materials
</commit_message>
<xml_diff>
--- a/bill_of_materials.xlsx
+++ b/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcdan\Projects\transponder_design_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E6558-7447-471E-8D98-0D45D9E8C716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED875ED-BD57-40F2-AF22-B985F0636EC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B2E5BA6A-386E-4787-A60C-02BD7F16E005}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -213,6 +213,51 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/4440</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/93395A173/</t>
+  </si>
+  <si>
+    <t>Receiver Case Screws</t>
+  </si>
+  <si>
+    <t>McMaster</t>
+  </si>
+  <si>
+    <t>M2.5x5 Flathead Screw (25 pack)</t>
+  </si>
+  <si>
+    <t>OLED Display Screws</t>
+  </si>
+  <si>
+    <t>M2x4 Socket Head Screw (100 pack)</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91292A004/</t>
+  </si>
+  <si>
+    <t>XBee Carrier Screws</t>
+  </si>
+  <si>
+    <t>M3x5 Socket Head Screw (100 pack)</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91292A110/</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Fasteners</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>3D Printing</t>
   </si>
 </sst>
 </file>
@@ -600,451 +645,592 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D4D62-A092-4F47-9ED6-9DF7F5561DD2}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="117.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="117.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4">
-        <f>E2*D2</f>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <f>F2*E2</f>
         <v>9.9499999999999993</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>4.95</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <f t="shared" ref="F3:F18" si="0">E3*D3</f>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G21" si="0">F3*E3</f>
         <v>4.95</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>17.5</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>2.95</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>2.95</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>10.95</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>10.95</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>0.95</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>42.9</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>42.9</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>20</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4.97</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.97</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="4">
+        <v>13.06</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>13.06</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3.84</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>3.84</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="5">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E23" s="4">
         <v>22</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="0"/>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
+        <f>F23*E23</f>
         <v>22</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="5">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4">
-        <v>7</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.59</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="4">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="4">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{CF31F703-DCC1-470C-854B-69CC35EC852B}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{0F1B1325-C083-4FD5-A404-EB65C16B0D67}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{DAD6B44F-6415-476B-A43C-802B42EEE934}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{35DF7111-C875-4964-820E-777DEE26C2F5}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{3F84900F-5F74-4CBC-B603-B3D09270102E}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{76B58BB1-DEA2-4B8B-8276-7DD157BB9982}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{0CA74C9E-197A-4ED9-B693-E4A2FE135431}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{F9D7EBC4-7652-4F0A-8859-70D0A35100F4}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{6AA2A10E-AE0B-4CDA-A478-AE929C206090}"/>
-    <hyperlink ref="G12" r:id="rId10" xr:uid="{58AF13F5-FDE2-494B-A844-4A643238E86A}"/>
-    <hyperlink ref="G13" r:id="rId11" xr:uid="{50556E95-DFA4-422E-B6F6-03BC9D550239}"/>
-    <hyperlink ref="G14" r:id="rId12" xr:uid="{63BAA9F7-E1F3-4215-9997-CE690D426D5B}"/>
-    <hyperlink ref="G15" r:id="rId13" xr:uid="{A36BEFDE-4FD5-4D88-9CCD-43531DFF0644}"/>
-    <hyperlink ref="G16" r:id="rId14" xr:uid="{7A26B210-A289-4662-AD02-66F9177F0DFC}"/>
-    <hyperlink ref="G17" r:id="rId15" xr:uid="{A2AE9A58-0EBA-4410-82BD-F81C748A0E3D}"/>
-    <hyperlink ref="G18" r:id="rId16" xr:uid="{D58BB629-8185-419C-82B1-B590F744E916}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{CF31F703-DCC1-470C-854B-69CC35EC852B}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{0F1B1325-C083-4FD5-A404-EB65C16B0D67}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{DAD6B44F-6415-476B-A43C-802B42EEE934}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{35DF7111-C875-4964-820E-777DEE26C2F5}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{3F84900F-5F74-4CBC-B603-B3D09270102E}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{76B58BB1-DEA2-4B8B-8276-7DD157BB9982}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{0CA74C9E-197A-4ED9-B693-E4A2FE135431}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{F9D7EBC4-7652-4F0A-8859-70D0A35100F4}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{6AA2A10E-AE0B-4CDA-A478-AE929C206090}"/>
+    <hyperlink ref="H23" r:id="rId10" xr:uid="{58AF13F5-FDE2-494B-A844-4A643238E86A}"/>
+    <hyperlink ref="H16" r:id="rId11" xr:uid="{50556E95-DFA4-422E-B6F6-03BC9D550239}"/>
+    <hyperlink ref="H17" r:id="rId12" xr:uid="{63BAA9F7-E1F3-4215-9997-CE690D426D5B}"/>
+    <hyperlink ref="H18" r:id="rId13" xr:uid="{A36BEFDE-4FD5-4D88-9CCD-43531DFF0644}"/>
+    <hyperlink ref="H19" r:id="rId14" xr:uid="{7A26B210-A289-4662-AD02-66F9177F0DFC}"/>
+    <hyperlink ref="H20" r:id="rId15" xr:uid="{A2AE9A58-0EBA-4410-82BD-F81C748A0E3D}"/>
+    <hyperlink ref="H21" r:id="rId16" xr:uid="{D58BB629-8185-419C-82B1-B590F744E916}"/>
+    <hyperlink ref="H14" r:id="rId17" xr:uid="{0103EBE4-7115-4EC2-886E-52F727175C69}"/>
+    <hyperlink ref="H13" r:id="rId18" xr:uid="{2E2793EB-0EDB-4EE2-96AD-A4CAD8B20946}"/>
+    <hyperlink ref="H12" r:id="rId19" xr:uid="{79D274FB-40DB-465F-9461-13A9A3E2AAB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>